<commit_message>
change language to ind
</commit_message>
<xml_diff>
--- a/assets/santri.xlsx
+++ b/assets/santri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\siks\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819DA306-D4BE-4AA5-AB3A-708564B8F943}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A30125D-0454-4873-A7FD-0557B7760C1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Nama Depan</t>
-  </si>
-  <si>
-    <t>Nama Belakang</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+  <si>
+    <t>Nama Lengkap</t>
+  </si>
+  <si>
+    <t>No Induk</t>
+  </si>
+  <si>
+    <t>NISN</t>
   </si>
   <si>
     <t>JK</t>
@@ -37,55 +40,118 @@
     <t>Tanggal Lahir</t>
   </si>
   <si>
+    <t>Agama</t>
+  </si>
+  <si>
+    <t>Status dlm Keluarga</t>
+  </si>
+  <si>
+    <t>Anak ke-</t>
+  </si>
+  <si>
     <t>Alamat</t>
   </si>
   <si>
-    <t>No Hp</t>
-  </si>
-  <si>
-    <t>Nama Ayah</t>
+    <t>Asal Sekolah</t>
+  </si>
+  <si>
+    <t>Diterima dikelas</t>
+  </si>
+  <si>
+    <t>Tgl diterima</t>
+  </si>
+  <si>
+    <t>Ayah</t>
   </si>
   <si>
     <t>Pekerjaan Ayah</t>
   </si>
   <si>
-    <t>Nama Ibu</t>
+    <t>Ibu</t>
   </si>
   <si>
     <t>Pekerjaan Ibu</t>
   </si>
   <si>
-    <t>Ahmad</t>
-  </si>
-  <si>
-    <t>Mustofa</t>
+    <t>Wali</t>
+  </si>
+  <si>
+    <t>Pekerjaan Wali</t>
+  </si>
+  <si>
+    <t>maman abdurahman</t>
   </si>
   <si>
     <t>M</t>
   </si>
   <si>
-    <t>Bogor</t>
-  </si>
-  <si>
-    <t>2005-07-09</t>
-  </si>
-  <si>
-    <t>Jl. soleh iskandar sebrang jalan baru no. 109</t>
-  </si>
-  <si>
-    <t>085712345678</t>
-  </si>
-  <si>
-    <t>Asep</t>
-  </si>
-  <si>
-    <t>Karyawan Swasta</t>
-  </si>
-  <si>
-    <t>Maemunah</t>
-  </si>
-  <si>
-    <t>Ibu Rumah Tangga</t>
+    <t>bogr</t>
+  </si>
+  <si>
+    <t>2020-08-04</t>
+  </si>
+  <si>
+    <t>adf</t>
+  </si>
+  <si>
+    <t>dfadf</t>
+  </si>
+  <si>
+    <t>afaf</t>
+  </si>
+  <si>
+    <t>dfsa</t>
+  </si>
+  <si>
+    <t>2020-08-14</t>
+  </si>
+  <si>
+    <t>dfafd</t>
+  </si>
+  <si>
+    <t>dfdfsf</t>
+  </si>
+  <si>
+    <t>adfas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aisayah </t>
+  </si>
+  <si>
+    <t>adsf</t>
+  </si>
+  <si>
+    <t>2020-08-02</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>adfs</t>
+  </si>
+  <si>
+    <t>dfasf</t>
+  </si>
+  <si>
+    <t>adfa</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>adfaf</t>
+  </si>
+  <si>
+    <t>afasf</t>
+  </si>
+  <si>
+    <t>afdadf</t>
+  </si>
+  <si>
+    <t>dafas</t>
+  </si>
+  <si>
+    <t>sadfa</t>
   </si>
 </sst>
 </file>
@@ -425,28 +491,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,40 +533,147 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>2342</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
       </c>
       <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>2345</v>
+      </c>
+      <c r="C3">
+        <v>134</v>
+      </c>
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
-        <v>21</v>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>